<commit_message>
codes zoeken probleem insp_det
</commit_message>
<xml_diff>
--- a/05_joris-behr/test.xlsx
+++ b/05_joris-behr/test.xlsx
@@ -607,106 +607,106 @@
         <v>39</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>28</v>
       </c>
       <c r="F2">
-        <v>454.19</v>
+        <v>452.53</v>
       </c>
       <c r="G2">
-        <v>10.71</v>
+        <v>10.69</v>
       </c>
       <c r="H2">
-        <v>19.01</v>
+        <v>18.94</v>
       </c>
       <c r="I2">
-        <v>1.07</v>
+        <v>1.27</v>
       </c>
       <c r="J2">
+        <v>0.11</v>
+      </c>
+      <c r="K2">
+        <v>4.75</v>
+      </c>
+      <c r="L2">
+        <v>0.72</v>
+      </c>
+      <c r="M2">
         <v>0.06</v>
-      </c>
-      <c r="K2">
-        <v>4.83</v>
-      </c>
-      <c r="L2">
-        <v>0.57</v>
-      </c>
-      <c r="M2">
-        <v>0.03</v>
       </c>
       <c r="N2">
         <v>14.9</v>
       </c>
       <c r="O2">
-        <v>0.96</v>
+        <v>1.09</v>
       </c>
       <c r="P2">
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="Q2">
-        <v>65.98</v>
+        <v>66.54000000000001</v>
       </c>
       <c r="R2">
-        <v>12.57</v>
+        <v>12.37</v>
       </c>
       <c r="S2">
-        <v>0.75</v>
+        <v>1.05</v>
       </c>
       <c r="T2">
         <v>4.74</v>
       </c>
       <c r="U2">
-        <v>0.82</v>
+        <v>0.78</v>
       </c>
       <c r="V2">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="W2">
+        <v>324.02</v>
+      </c>
+      <c r="X2">
+        <v>27.51</v>
+      </c>
+      <c r="Y2">
+        <v>2.34</v>
+      </c>
+      <c r="Z2">
+        <v>23.53</v>
+      </c>
+      <c r="AA2">
+        <v>1.66</v>
+      </c>
+      <c r="AB2">
+        <v>0.14</v>
+      </c>
+      <c r="AC2">
+        <v>19.72</v>
+      </c>
+      <c r="AD2">
+        <v>1.51</v>
+      </c>
+      <c r="AE2">
+        <v>0.13</v>
+      </c>
+      <c r="AF2">
+        <v>20.78</v>
+      </c>
+      <c r="AG2">
+        <v>1.59</v>
+      </c>
+      <c r="AH2">
+        <v>0.13</v>
+      </c>
+      <c r="AI2">
+        <v>24.73</v>
+      </c>
+      <c r="AJ2">
+        <v>0.58</v>
+      </c>
+      <c r="AK2">
         <v>0.05</v>
-      </c>
-      <c r="W2">
-        <v>323.67</v>
-      </c>
-      <c r="X2">
-        <v>26.63</v>
-      </c>
-      <c r="Y2">
-        <v>1.6</v>
-      </c>
-      <c r="Z2">
-        <v>23.6</v>
-      </c>
-      <c r="AA2">
-        <v>1.54</v>
-      </c>
-      <c r="AB2">
-        <v>0.09</v>
-      </c>
-      <c r="AC2">
-        <v>19.81</v>
-      </c>
-      <c r="AD2">
-        <v>1.24</v>
-      </c>
-      <c r="AE2">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="AF2">
-        <v>20.68</v>
-      </c>
-      <c r="AG2">
-        <v>1.26</v>
-      </c>
-      <c r="AH2">
-        <v>0.08</v>
-      </c>
-      <c r="AI2">
-        <v>24.71</v>
-      </c>
-      <c r="AJ2">
-        <v>0.55</v>
-      </c>
-      <c r="AK2">
-        <v>0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commenting most graphs for faster code running
</commit_message>
<xml_diff>
--- a/05_joris-behr/test.xlsx
+++ b/05_joris-behr/test.xlsx
@@ -127,7 +127,7 @@
     <t>SE Transpulmonary Pressure Swing</t>
   </si>
   <si>
-    <t>5__211029094903_Waves_001.txt</t>
+    <t>1__211006132800_Waves_001.txt</t>
   </si>
   <si>
     <t>234</t>
@@ -607,106 +607,106 @@
         <v>39</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E2">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="F2">
-        <v>452.53</v>
+        <v>513.08</v>
       </c>
       <c r="G2">
-        <v>10.69</v>
+        <v>7.71</v>
       </c>
       <c r="H2">
-        <v>18.94</v>
+        <v>5.78</v>
       </c>
       <c r="I2">
-        <v>1.27</v>
+        <v>0.79</v>
       </c>
       <c r="J2">
-        <v>0.11</v>
+        <v>0.06</v>
       </c>
       <c r="K2">
-        <v>4.75</v>
+        <v>3.46</v>
       </c>
       <c r="L2">
-        <v>0.72</v>
+        <v>0.71</v>
       </c>
       <c r="M2">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="N2">
-        <v>14.9</v>
+        <v>3.86</v>
       </c>
       <c r="O2">
-        <v>1.09</v>
+        <v>0.55</v>
       </c>
       <c r="P2">
+        <v>0.04</v>
+      </c>
+      <c r="Q2">
+        <v>44.63</v>
+      </c>
+      <c r="R2">
+        <v>15.41</v>
+      </c>
+      <c r="S2">
+        <v>1.15</v>
+      </c>
+      <c r="T2">
+        <v>2.75</v>
+      </c>
+      <c r="U2">
+        <v>0.6</v>
+      </c>
+      <c r="V2">
+        <v>0.04</v>
+      </c>
+      <c r="W2">
+        <v>132.64</v>
+      </c>
+      <c r="X2">
+        <v>26.53</v>
+      </c>
+      <c r="Y2">
+        <v>1.97</v>
+      </c>
+      <c r="Z2">
+        <v>8.35</v>
+      </c>
+      <c r="AA2">
+        <v>1.16</v>
+      </c>
+      <c r="AB2">
         <v>0.09</v>
       </c>
-      <c r="Q2">
-        <v>66.54000000000001</v>
-      </c>
-      <c r="R2">
-        <v>12.37</v>
-      </c>
-      <c r="S2">
-        <v>1.05</v>
-      </c>
-      <c r="T2">
-        <v>4.74</v>
-      </c>
-      <c r="U2">
-        <v>0.78</v>
-      </c>
-      <c r="V2">
+      <c r="AC2">
+        <v>7.27</v>
+      </c>
+      <c r="AD2">
+        <v>1.03</v>
+      </c>
+      <c r="AE2">
+        <v>0.08</v>
+      </c>
+      <c r="AF2">
+        <v>11.36</v>
+      </c>
+      <c r="AG2">
+        <v>2.3</v>
+      </c>
+      <c r="AH2">
+        <v>0.17</v>
+      </c>
+      <c r="AI2">
+        <v>17.43</v>
+      </c>
+      <c r="AJ2">
+        <v>0.99</v>
+      </c>
+      <c r="AK2">
         <v>0.07000000000000001</v>
-      </c>
-      <c r="W2">
-        <v>324.02</v>
-      </c>
-      <c r="X2">
-        <v>27.51</v>
-      </c>
-      <c r="Y2">
-        <v>2.34</v>
-      </c>
-      <c r="Z2">
-        <v>23.53</v>
-      </c>
-      <c r="AA2">
-        <v>1.66</v>
-      </c>
-      <c r="AB2">
-        <v>0.14</v>
-      </c>
-      <c r="AC2">
-        <v>19.72</v>
-      </c>
-      <c r="AD2">
-        <v>1.51</v>
-      </c>
-      <c r="AE2">
-        <v>0.13</v>
-      </c>
-      <c r="AF2">
-        <v>20.78</v>
-      </c>
-      <c r="AG2">
-        <v>1.59</v>
-      </c>
-      <c r="AH2">
-        <v>0.13</v>
-      </c>
-      <c r="AI2">
-        <v>24.73</v>
-      </c>
-      <c r="AJ2">
-        <v>0.58</v>
-      </c>
-      <c r="AK2">
-        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created breath_ham + ham_vs_script
</commit_message>
<xml_diff>
--- a/05_joris-behr/test.xlsx
+++ b/05_joris-behr/test.xlsx
@@ -127,7 +127,7 @@
     <t>SE Transpulmonary Pressure Swing</t>
   </si>
   <si>
-    <t>W_Hamilton-C6__220321153431_Waves_001.txt</t>
+    <t>1__211006132800_Waves_001.txt</t>
   </si>
   <si>
     <t>234</t>
@@ -607,106 +607,106 @@
         <v>39</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F2">
-        <v>535.48</v>
+        <v>510.58</v>
       </c>
       <c r="G2">
-        <v>10.28</v>
+        <v>7.71</v>
       </c>
       <c r="H2">
-        <v>13.41</v>
+        <v>5.79</v>
       </c>
       <c r="I2">
-        <v>3.48</v>
+        <v>0.5</v>
       </c>
       <c r="J2">
-        <v>0.22</v>
+        <v>0.06</v>
       </c>
       <c r="K2">
-        <v>5.22</v>
+        <v>3.56</v>
       </c>
       <c r="L2">
-        <v>1.76</v>
+        <v>0.33</v>
       </c>
       <c r="M2">
+        <v>0.04</v>
+      </c>
+      <c r="N2">
+        <v>3.89</v>
+      </c>
+      <c r="O2">
+        <v>0.34</v>
+      </c>
+      <c r="P2">
+        <v>0.04</v>
+      </c>
+      <c r="Q2">
+        <v>42.83</v>
+      </c>
+      <c r="R2">
+        <v>7.14</v>
+      </c>
+      <c r="S2">
+        <v>0.91</v>
+      </c>
+      <c r="T2">
+        <v>2.79</v>
+      </c>
+      <c r="U2">
+        <v>0.37</v>
+      </c>
+      <c r="V2">
+        <v>0.05</v>
+      </c>
+      <c r="W2">
+        <v>131.24</v>
+      </c>
+      <c r="X2">
+        <v>12.59</v>
+      </c>
+      <c r="Y2">
+        <v>1.61</v>
+      </c>
+      <c r="Z2">
+        <v>8.41</v>
+      </c>
+      <c r="AA2">
+        <v>0.8</v>
+      </c>
+      <c r="AB2">
+        <v>0.1</v>
+      </c>
+      <c r="AC2">
+        <v>7.44</v>
+      </c>
+      <c r="AD2">
+        <v>0.64</v>
+      </c>
+      <c r="AE2">
+        <v>0.08</v>
+      </c>
+      <c r="AF2">
+        <v>11.1</v>
+      </c>
+      <c r="AG2">
+        <v>0.46</v>
+      </c>
+      <c r="AH2">
+        <v>0.06</v>
+      </c>
+      <c r="AI2">
+        <v>17.34</v>
+      </c>
+      <c r="AJ2">
+        <v>0.85</v>
+      </c>
+      <c r="AK2">
         <v>0.11</v>
-      </c>
-      <c r="N2">
-        <v>8.06</v>
-      </c>
-      <c r="O2">
-        <v>2.83</v>
-      </c>
-      <c r="P2">
-        <v>0.18</v>
-      </c>
-      <c r="Q2">
-        <v>56.72</v>
-      </c>
-      <c r="R2">
-        <v>14.93</v>
-      </c>
-      <c r="S2">
-        <v>0.96</v>
-      </c>
-      <c r="T2">
-        <v>4.2</v>
-      </c>
-      <c r="U2">
-        <v>1.29</v>
-      </c>
-      <c r="V2">
-        <v>0.08</v>
-      </c>
-      <c r="W2">
-        <v>317.39</v>
-      </c>
-      <c r="X2">
-        <v>62.29</v>
-      </c>
-      <c r="Y2">
-        <v>3.99</v>
-      </c>
-      <c r="Z2">
-        <v>15.9</v>
-      </c>
-      <c r="AA2">
-        <v>4.13</v>
-      </c>
-      <c r="AB2">
-        <v>0.26</v>
-      </c>
-      <c r="AC2">
-        <v>13.22</v>
-      </c>
-      <c r="AD2">
-        <v>3.54</v>
-      </c>
-      <c r="AE2">
-        <v>0.23</v>
-      </c>
-      <c r="AF2">
-        <v>19.1</v>
-      </c>
-      <c r="AG2">
-        <v>1.97</v>
-      </c>
-      <c r="AH2">
-        <v>0.13</v>
-      </c>
-      <c r="AI2">
-        <v>15.34</v>
-      </c>
-      <c r="AJ2">
-        <v>2.12</v>
-      </c>
-      <c r="AK2">
-        <v>0.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimizing finding start insp with breath no data
</commit_message>
<xml_diff>
--- a/05_joris-behr/test.xlsx
+++ b/05_joris-behr/test.xlsx
@@ -127,7 +127,7 @@
     <t>SE Transpulmonary Pressure Swing</t>
   </si>
   <si>
-    <t>Waves_005.txt</t>
+    <t>Waves_009.txt</t>
   </si>
   <si>
     <t>234</t>
@@ -607,106 +607,106 @@
         <v>39</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="E2">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F2">
-        <v>432.12</v>
+        <v>449.43</v>
       </c>
       <c r="G2">
-        <v>10.69</v>
+        <v>7.54</v>
       </c>
       <c r="H2">
-        <v>17.73</v>
+        <v>4.9</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>3.62</v>
       </c>
       <c r="J2">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="K2">
-        <v>4.48</v>
+        <v>3.38</v>
       </c>
       <c r="L2">
-        <v>0.39</v>
+        <v>2.1</v>
       </c>
       <c r="M2">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="N2">
-        <v>13.83</v>
+        <v>2.25</v>
       </c>
       <c r="O2">
-        <v>0.76</v>
+        <v>0.82</v>
       </c>
       <c r="P2">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="Q2">
-        <v>62.75</v>
+        <v>482.29</v>
       </c>
       <c r="R2">
-        <v>10.69</v>
+        <v>540.05</v>
       </c>
       <c r="S2">
-        <v>0.65</v>
+        <v>14.68</v>
       </c>
       <c r="T2">
-        <v>4.35</v>
+        <v>14.07</v>
       </c>
       <c r="U2">
-        <v>0.66</v>
+        <v>18.61</v>
       </c>
       <c r="V2">
-        <v>0.04</v>
+        <v>0.51</v>
       </c>
       <c r="W2">
-        <v>313.17</v>
+        <v>526.6</v>
       </c>
       <c r="X2">
-        <v>24.12</v>
+        <v>596.0700000000001</v>
       </c>
       <c r="Y2">
-        <v>1.46</v>
+        <v>16.2</v>
       </c>
       <c r="Z2">
-        <v>21.94</v>
+        <v>14.31</v>
       </c>
       <c r="AA2">
-        <v>1.36</v>
+        <v>16.74</v>
       </c>
       <c r="AB2">
-        <v>0.08</v>
+        <v>0.46</v>
       </c>
       <c r="AC2">
-        <v>18.34</v>
+        <v>3.17</v>
       </c>
       <c r="AD2">
-        <v>1.05</v>
+        <v>1.3</v>
       </c>
       <c r="AE2">
         <v>0.06</v>
       </c>
       <c r="AF2">
-        <v>21.69</v>
+        <v>8.93</v>
       </c>
       <c r="AG2">
-        <v>1.15</v>
+        <v>3.52</v>
       </c>
       <c r="AH2">
-        <v>0.07000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="AI2">
-        <v>24.53</v>
+        <v>13.46</v>
       </c>
       <c r="AJ2">
-        <v>0.53</v>
+        <v>4.92</v>
       </c>
       <c r="AK2">
-        <v>0.03</v>
+        <v>0.13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented hamilton breath detection
</commit_message>
<xml_diff>
--- a/05_joris-behr/test.xlsx
+++ b/05_joris-behr/test.xlsx
@@ -127,7 +127,7 @@
     <t>SE Transpulmonary Pressure Swing</t>
   </si>
   <si>
-    <t>Waves_001.txt</t>
+    <t>Waves_009.txt</t>
   </si>
   <si>
     <t>234</t>
@@ -607,106 +607,106 @@
         <v>39</v>
       </c>
       <c r="D2">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="E2">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F2">
-        <v>513.08</v>
+        <v>452.55</v>
       </c>
       <c r="G2">
-        <v>7.71</v>
+        <v>7.54</v>
       </c>
       <c r="H2">
-        <v>5.78</v>
+        <v>4.67</v>
       </c>
       <c r="I2">
-        <v>0.79</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>3.46</v>
+        <v>4.19</v>
       </c>
       <c r="L2">
-        <v>0.71</v>
+        <v>3.13</v>
       </c>
       <c r="M2">
-        <v>0.05</v>
+        <v>0.09</v>
       </c>
       <c r="N2">
-        <v>3.86</v>
+        <v>2.13</v>
       </c>
       <c r="O2">
-        <v>0.55</v>
+        <v>1.16</v>
       </c>
       <c r="P2">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="Q2">
-        <v>44.63</v>
+        <v>56.8</v>
       </c>
       <c r="R2">
-        <v>15.41</v>
+        <v>33.51</v>
       </c>
       <c r="S2">
-        <v>1.15</v>
+        <v>0.93</v>
       </c>
       <c r="T2">
-        <v>2.75</v>
+        <v>2.12</v>
       </c>
       <c r="U2">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>132.64</v>
+        <v>94.87</v>
       </c>
       <c r="X2">
-        <v>26.53</v>
+        <v>38.18</v>
       </c>
       <c r="Y2">
-        <v>1.97</v>
+        <v>1.05</v>
       </c>
       <c r="Z2">
-        <v>8.35</v>
+        <v>6.56</v>
       </c>
       <c r="AA2">
-        <v>1.16</v>
+        <v>0</v>
       </c>
       <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>3.89</v>
+      </c>
+      <c r="AD2">
+        <v>2.53</v>
+      </c>
+      <c r="AE2">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="AF2">
+        <v>7.83</v>
+      </c>
+      <c r="AG2">
+        <v>2.99</v>
+      </c>
+      <c r="AH2">
+        <v>0.08</v>
+      </c>
+      <c r="AI2">
+        <v>11.46</v>
+      </c>
+      <c r="AJ2">
+        <v>3.4</v>
+      </c>
+      <c r="AK2">
         <v>0.09</v>
-      </c>
-      <c r="AC2">
-        <v>7.27</v>
-      </c>
-      <c r="AD2">
-        <v>1.03</v>
-      </c>
-      <c r="AE2">
-        <v>0.08</v>
-      </c>
-      <c r="AF2">
-        <v>11.36</v>
-      </c>
-      <c r="AG2">
-        <v>2.3</v>
-      </c>
-      <c r="AH2">
-        <v>0.17</v>
-      </c>
-      <c r="AI2">
-        <v>17.43</v>
-      </c>
-      <c r="AJ2">
-        <v>0.99</v>
-      </c>
-      <c r="AK2">
-        <v>0.07000000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start new method using diff and flowshift
</commit_message>
<xml_diff>
--- a/05_joris-behr/test.xlsx
+++ b/05_joris-behr/test.xlsx
@@ -127,7 +127,7 @@
     <t>SE Transpulmonary Pressure Swing</t>
   </si>
   <si>
-    <t>Waves_009.txt</t>
+    <t>Waves_005.txt</t>
   </si>
   <si>
     <t>234</t>
@@ -607,19 +607,19 @@
         <v>39</v>
       </c>
       <c r="D2">
-        <v>72</v>
+        <v>147</v>
       </c>
       <c r="E2">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F2">
-        <v>452.55</v>
+        <v>436.61</v>
       </c>
       <c r="G2">
-        <v>7.54</v>
+        <v>10.69</v>
       </c>
       <c r="H2">
-        <v>4.67</v>
+        <v>20.28</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -628,34 +628,34 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>4.19</v>
+        <v>4.67</v>
       </c>
       <c r="L2">
-        <v>3.13</v>
+        <v>0.6</v>
       </c>
       <c r="M2">
-        <v>0.09</v>
+        <v>0.01</v>
       </c>
       <c r="N2">
-        <v>2.13</v>
+        <v>14.38</v>
       </c>
       <c r="O2">
-        <v>1.16</v>
+        <v>1.02</v>
       </c>
       <c r="P2">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="Q2">
-        <v>56.8</v>
+        <v>66.20999999999999</v>
       </c>
       <c r="R2">
-        <v>33.51</v>
+        <v>12.7</v>
       </c>
       <c r="S2">
-        <v>0.93</v>
+        <v>0.2</v>
       </c>
       <c r="T2">
-        <v>2.12</v>
+        <v>5.53</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -664,16 +664,16 @@
         <v>0</v>
       </c>
       <c r="W2">
-        <v>94.87</v>
+        <v>333.3</v>
       </c>
       <c r="X2">
-        <v>38.18</v>
+        <v>28.31</v>
       </c>
       <c r="Y2">
-        <v>1.05</v>
+        <v>0.44</v>
       </c>
       <c r="Z2">
-        <v>6.56</v>
+        <v>25.29</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -682,31 +682,31 @@
         <v>0</v>
       </c>
       <c r="AC2">
-        <v>3.89</v>
+        <v>19.07</v>
       </c>
       <c r="AD2">
-        <v>2.53</v>
+        <v>1.39</v>
       </c>
       <c r="AE2">
-        <v>0.07000000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="AF2">
-        <v>7.83</v>
+        <v>21.67</v>
       </c>
       <c r="AG2">
-        <v>2.99</v>
+        <v>1.76</v>
       </c>
       <c r="AH2">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
       <c r="AI2">
-        <v>11.46</v>
+        <v>24.45</v>
       </c>
       <c r="AJ2">
-        <v>3.4</v>
+        <v>0.74</v>
       </c>
       <c r="AK2">
-        <v>0.09</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding correlations to statistics
</commit_message>
<xml_diff>
--- a/05_joris-behr/test.xlsx
+++ b/05_joris-behr/test.xlsx
@@ -127,7 +127,7 @@
     <t>SE Transpulmonary Pressure Swing</t>
   </si>
   <si>
-    <t>Waves_003.txt</t>
+    <t>Waves_011.txt</t>
   </si>
   <si>
     <t>234</t>
@@ -607,19 +607,19 @@
         <v>39</v>
       </c>
       <c r="D2">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="E2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2">
-        <v>310.01</v>
+        <v>413.07</v>
       </c>
       <c r="G2">
-        <v>5.08</v>
+        <v>10.27</v>
       </c>
       <c r="H2">
-        <v>4.05</v>
+        <v>14.67</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -628,34 +628,34 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>4.41</v>
+        <v>9.75</v>
       </c>
       <c r="L2">
-        <v>1.16</v>
+        <v>1.47</v>
       </c>
       <c r="M2">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="N2">
-        <v>1.35</v>
+        <v>8.59</v>
       </c>
       <c r="O2">
-        <v>0.44</v>
+        <v>1.33</v>
       </c>
       <c r="P2">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="Q2">
-        <v>102.17</v>
+        <v>142.93</v>
       </c>
       <c r="R2">
-        <v>22.44</v>
+        <v>29.44</v>
       </c>
       <c r="S2">
-        <v>0.98</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="T2">
-        <v>4.3</v>
+        <v>7.69</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -664,16 +664,16 @@
         <v>0</v>
       </c>
       <c r="W2">
-        <v>181.25</v>
+        <v>326.77</v>
       </c>
       <c r="X2">
-        <v>31.2</v>
+        <v>37.55</v>
       </c>
       <c r="Y2">
-        <v>1.36</v>
+        <v>1.03</v>
       </c>
       <c r="Z2">
-        <v>8.19</v>
+        <v>21.88</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -682,31 +682,31 @@
         <v>0</v>
       </c>
       <c r="AC2">
-        <v>5.77</v>
+        <v>18.36</v>
       </c>
       <c r="AD2">
-        <v>1.34</v>
+        <v>2.22</v>
       </c>
       <c r="AE2">
         <v>0.06</v>
       </c>
       <c r="AF2">
-        <v>11.68</v>
+        <v>22.48</v>
       </c>
       <c r="AG2">
-        <v>2.03</v>
+        <v>2.07</v>
       </c>
       <c r="AH2">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="AI2">
-        <v>14.93</v>
+        <v>25.28</v>
       </c>
       <c r="AJ2">
-        <v>1.75</v>
+        <v>1.9</v>
       </c>
       <c r="AK2">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>